<commit_message>
EPBDS-8933 Validation message is presented for spreadsheets with the different business versions, if cells have different names
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7313_SR_SimplifiedRef_more_tests.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7313_SR_SimplifiedRef_more_tests.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7632852F-96C8-4181-BFE7-1EA9A615DCE4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="27795" windowHeight="10230"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="82">
   <si>
     <t>Spreadsheet SpreadsheetResult mySpr(Integer a)</t>
   </si>
@@ -51,24 +57,12 @@
     <t>=mySpr2(a).$Step1</t>
   </si>
   <si>
-    <t>SmartRules Integer mySmart2(Integer a)</t>
-  </si>
-  <si>
-    <t>=mySpr(a).$Values</t>
-  </si>
-  <si>
-    <t>=mySpr2(a).$Values</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test mySmart mySmartTest </t>
   </si>
   <si>
     <t>_res_</t>
   </si>
   <si>
-    <t xml:space="preserve">Test mySmart2 mySmart2Test </t>
-  </si>
-  <si>
     <t>=mySpr(a)</t>
   </si>
   <si>
@@ -123,15 +117,9 @@
     <t>Test  mySmartInputSR  mySmartInputSRtest</t>
   </si>
   <si>
-    <t>Test  mySmartInputSR  mySmartInputSRtest2</t>
-  </si>
-  <si>
     <t>a.$Values$Step1</t>
   </si>
   <si>
-    <t>a.$Values</t>
-  </si>
-  <si>
     <t>Spreadsheet SpreadsheetResult mySprTrenarOp(Integer a)</t>
   </si>
   <si>
@@ -183,12 +171,6 @@
     <t>SmartRules Integer mySmartotherSyntx(Integer a)</t>
   </si>
   <si>
-    <t>=$Values(mySpr2(a))</t>
-  </si>
-  <si>
-    <t>_res_.$someStep2.$Values</t>
-  </si>
-  <si>
     <t>=$Step1(mySpr(a))</t>
   </si>
   <si>
@@ -240,9 +222,6 @@
     <t>Test  mySmartInputSR2  mySmartInputSR2test</t>
   </si>
   <si>
-    <t>Test  mySmartInputSR2  mySmartInputSR2test2</t>
-  </si>
-  <si>
     <t>Trenary Operations</t>
   </si>
   <si>
@@ -286,12 +265,15 @@
   </si>
   <si>
     <t>109, 110, 200</t>
+  </si>
+  <si>
+    <t>_res_.$someStep2.$Step1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -415,8 +397,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Linked Cell" xfId="1" builtinId="24"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Связанная ячейка" xfId="1" builtinId="24"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -443,7 +425,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -452,14 +434,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -497,9 +482,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -532,9 +517,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -567,9 +569,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -742,11 +761,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P104"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:R110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,7 +782,7 @@
   <sheetData>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -813,17 +832,24 @@
         <v>5</v>
       </c>
     </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+    </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
-      <c r="I13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
@@ -833,13 +859,11 @@
       <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
@@ -849,17 +873,13 @@
         <v>20</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="3">
-        <v>1</v>
-      </c>
-      <c r="J15" s="3">
-        <v>20</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
@@ -871,53 +891,55 @@
       <c r="D16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="3">
-        <v>20</v>
-      </c>
-      <c r="J16" s="3">
-        <v>30</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C18" s="10"/>
-      <c r="I18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" s="10"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
@@ -926,12 +948,11 @@
       <c r="C21" s="3">
         <v>23</v>
       </c>
-      <c r="I21" s="3">
-        <v>19</v>
-      </c>
-      <c r="J21" s="3">
-        <v>23</v>
-      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
@@ -940,24 +961,29 @@
       <c r="C22" s="3">
         <v>26</v>
       </c>
-      <c r="I22" s="3">
-        <v>20</v>
-      </c>
-      <c r="J22" s="3">
-        <v>26</v>
-      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="7"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
-      <c r="I25" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
+      <c r="I25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="13"/>
+      <c r="K25" s="7"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
@@ -971,11 +997,9 @@
         <v>8</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="K26" s="7"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
@@ -985,17 +1009,15 @@
         <v>20</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="K27" s="7"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
@@ -1005,7 +1027,7 @@
         <v>30</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I28" s="3">
         <v>19</v>
@@ -1013,9 +1035,7 @@
       <c r="J28" s="3">
         <v>23</v>
       </c>
-      <c r="K28" s="3">
-        <v>23</v>
-      </c>
+      <c r="K28" s="7"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I29" s="3">
@@ -1024,23 +1044,21 @@
       <c r="J29" s="3">
         <v>124</v>
       </c>
-      <c r="K29" s="3">
-        <v>124</v>
-      </c>
+      <c r="K29" s="7"/>
     </row>
     <row r="30" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
+      <c r="K30" s="7"/>
     </row>
     <row r="31" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-    </row>
-    <row r="33" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K31" s="7"/>
+    </row>
+    <row r="33" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1050,157 +1068,171 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="13"/>
       <c r="I35" s="11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="13"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F36" s="10"/>
       <c r="I36" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L36" s="10"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F37" s="10"/>
       <c r="I37" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J37" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="L37" s="10"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F39" s="10"/>
       <c r="I39" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="L39" s="10"/>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B43" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="J43" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K43" s="10"/>
-      <c r="O43" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="P43" s="10"/>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="3" t="s">
         <v>9</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O44" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="P44" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="7"/>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
         <v>20</v>
       </c>
@@ -1211,19 +1243,18 @@
         <v>5</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O45" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="P45" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
         <v>40</v>
       </c>
@@ -1239,78 +1270,105 @@
       <c r="K46" s="3">
         <v>5</v>
       </c>
-      <c r="O46" s="3">
-        <v>25</v>
-      </c>
-      <c r="P46" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
       <c r="J47" s="3">
         <v>45</v>
       </c>
       <c r="K47" s="3">
         <v>6</v>
       </c>
-      <c r="O47" s="3">
-        <v>45</v>
-      </c>
-      <c r="P47" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="7"/>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="7"/>
+      <c r="Q49" s="7"/>
+      <c r="R49" s="7"/>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C50" s="10"/>
       <c r="J50" s="10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J51" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7"/>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B52" s="3">
         <v>20</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="N52" s="7"/>
+      <c r="O52" s="7"/>
+      <c r="P52" s="7"/>
+      <c r="Q52" s="7"/>
+      <c r="R52" s="7"/>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B53" s="3">
         <v>40</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="J53" s="3">
         <v>20</v>
@@ -1321,8 +1379,13 @@
       <c r="L53" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N53" s="7"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="7"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="7"/>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
       <c r="J54" s="3">
         <v>40</v>
       </c>
@@ -1332,27 +1395,28 @@
       <c r="L54" s="3">
         <v>44</v>
       </c>
-    </row>
-    <row r="55" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="7"/>
+    </row>
+    <row r="55" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
       <c r="I56" s="6"/>
       <c r="J56" s="10" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="K56" s="10"/>
-      <c r="O56" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="P56" s="10"/>
-    </row>
-    <row r="57" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="3" t="s">
@@ -1360,19 +1424,13 @@
       </c>
       <c r="I57" s="6"/>
       <c r="J57" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O57" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="P57" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="3">
         <v>20</v>
       </c>
@@ -1384,19 +1442,13 @@
       </c>
       <c r="I58" s="6"/>
       <c r="J58" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O58" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="P58" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="3">
         <v>40</v>
       </c>
@@ -1413,14 +1465,8 @@
       <c r="K59" s="3">
         <v>5</v>
       </c>
-      <c r="O59" s="3">
-        <v>25</v>
-      </c>
-      <c r="P59" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I60" s="6"/>
       <c r="J60" s="3">
         <v>45</v>
@@ -1428,54 +1474,46 @@
       <c r="K60" s="3">
         <v>6</v>
       </c>
-      <c r="O60" s="3">
-        <v>45</v>
-      </c>
-      <c r="P60" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
-      <c r="O61" s="6"/>
-      <c r="P61" s="6"/>
-    </row>
-    <row r="62" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
       <c r="O62" s="6"/>
       <c r="P62" s="6"/>
     </row>
-    <row r="63" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
       <c r="I63" s="10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="J63" s="10"/>
       <c r="K63" s="6"/>
       <c r="O63" s="6"/>
       <c r="P63" s="6"/>
     </row>
-    <row r="64" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D64" s="10"/>
       <c r="I64" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K64" s="6"/>
       <c r="O64" s="6"/>
@@ -1486,16 +1524,16 @@
         <v>1</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I65" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K65" s="6"/>
       <c r="O65" s="6"/>
@@ -1506,10 +1544,10 @@
         <v>2</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I66" s="3">
         <v>1</v>
@@ -1535,7 +1573,7 @@
     </row>
     <row r="69" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -1548,11 +1586,11 @@
     <row r="70" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B72" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C72" s="10"/>
       <c r="I72" s="10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J72" s="10"/>
     </row>
@@ -1567,29 +1605,29 @@
         <v>8</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I74" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I75" s="3">
         <v>100</v>
@@ -1600,7 +1638,7 @@
     </row>
     <row r="78" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
@@ -1613,11 +1651,11 @@
     <row r="79" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="80" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B80" s="10" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C80" s="10"/>
       <c r="I80" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J80" s="10"/>
       <c r="K80" s="10"/>
@@ -1631,45 +1669,45 @@
         <v>2</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="L81" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D82" s="1"/>
       <c r="I82" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="L82" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D83" s="1"/>
       <c r="I83" s="3">
@@ -1689,7 +1727,7 @@
     <row r="86" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="87" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I87" s="10" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="J87" s="10"/>
       <c r="K87" s="10"/>
@@ -1697,20 +1735,20 @@
     </row>
     <row r="88" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="10" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C88" s="10"/>
       <c r="I88" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="L88" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1721,24 +1759,24 @@
         <v>2</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="K89" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="L89" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I90" s="3">
         <v>5</v>
@@ -1750,22 +1788,22 @@
         <v>96</v>
       </c>
       <c r="L90" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="91" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="92" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="93" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="96" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B96" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
@@ -1775,19 +1813,19 @@
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
     </row>
-    <row r="97" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B98" s="10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C98" s="10"/>
       <c r="D98" s="10"/>
       <c r="I98" s="10" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J98" s="10"/>
     </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B99" s="10" t="s">
         <v>8</v>
       </c>
@@ -1797,10 +1835,10 @@
         <v>8</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B100" s="3">
         <v>1</v>
       </c>
@@ -1808,24 +1846,24 @@
         <v>20</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I100" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J100" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B101" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C101" s="3">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I101" s="3">
         <v>19</v>
@@ -1834,94 +1872,145 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B102" s="3">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C102" s="3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I102" s="3">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="J102" s="3">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B103" s="3">
-        <v>50</v>
-      </c>
-      <c r="C103" s="3">
-        <v>60</v>
-      </c>
-      <c r="D103" s="4" t="s">
-        <v>63</v>
-      </c>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A103" s="7"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="7"/>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
       <c r="I103" s="3">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="J103" s="3">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I104" s="3">
-        <v>51</v>
-      </c>
-      <c r="J104" s="3">
         <v>55</v>
       </c>
     </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" s="7"/>
+      <c r="B104" s="7"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+      <c r="H104" s="7"/>
+      <c r="I104" s="7"/>
+      <c r="J104" s="7"/>
+      <c r="K104" s="7"/>
+      <c r="L104" s="7"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A105" s="7"/>
+      <c r="B105" s="7"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7"/>
+      <c r="H105" s="7"/>
+      <c r="I105" s="7"/>
+      <c r="J105" s="7"/>
+      <c r="K105" s="7"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A106" s="7"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="7"/>
+      <c r="E106" s="7"/>
+      <c r="H106" s="7"/>
+      <c r="I106" s="7"/>
+      <c r="J106" s="7"/>
+      <c r="K106" s="7"/>
+      <c r="L106" s="7"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A107" s="7"/>
+      <c r="B107" s="7"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="7"/>
+      <c r="E107" s="7"/>
+      <c r="H107" s="7"/>
+      <c r="I107" s="7"/>
+      <c r="J107" s="7"/>
+      <c r="K107" s="7"/>
+      <c r="L107" s="7"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H108" s="7"/>
+      <c r="I108" s="7"/>
+      <c r="J108" s="7"/>
+      <c r="K108" s="7"/>
+      <c r="L108" s="7"/>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H109" s="7"/>
+      <c r="I109" s="7"/>
+      <c r="J109" s="7"/>
+      <c r="K109" s="7"/>
+      <c r="L109" s="7"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H110" s="7"/>
+      <c r="I110" s="7"/>
+      <c r="J110" s="7"/>
+      <c r="K110" s="7"/>
+      <c r="L110" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="39">
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K39:L39"/>
     <mergeCell ref="I87:L87"/>
+    <mergeCell ref="I80:L80"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="J50:L50"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="I35:L35"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I98:J98"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E36:F36"/>
     <mergeCell ref="B99:C99"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="I14:J14"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="B80:C80"/>
-    <mergeCell ref="I80:L80"/>
     <mergeCell ref="B98:D98"/>
-    <mergeCell ref="I98:J98"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="E36:F36"/>
     <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="O43:P43"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="J50:L50"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="O56:P56"/>
-    <mergeCell ref="I35:L35"/>
     <mergeCell ref="B63:D63"/>
     <mergeCell ref="C64:D64"/>
     <mergeCell ref="I63:J63"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K39:L39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1929,7 +2018,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1941,7 +2030,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
EPBDS-7313 Add possibility to use simplified reference to SR cells of an external SR (not current). Fix - should be the same behaviour for all parts of the system.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7313_SR_SimplifiedRef_more_tests.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7313_SR_SimplifiedRef_more_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7632852F-96C8-4181-BFE7-1EA9A615DCE4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712C4926-C9A6-4606-BCDA-79B7BB59543B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3740" yWindow="4350" windowWidth="26450" windowHeight="14960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="81">
   <si>
     <t>Spreadsheet SpreadsheetResult mySpr(Integer a)</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>_res_.$Step1</t>
-  </si>
-  <si>
-    <t>_res_.$Values</t>
   </si>
   <si>
     <t>Conditions</t>
@@ -764,25 +761,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:R110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="K68" sqref="K68"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="L62" sqref="L62:L63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="47.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38.85546875" customWidth="1"/>
-    <col min="9" max="9" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="29.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="32.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="47.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="38.81640625" customWidth="1"/>
+    <col min="9" max="9" width="26.26953125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="25.26953125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.81640625" customWidth="1"/>
+    <col min="12" max="12" width="29.54296875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="32.26953125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -792,8 +789,8 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" s="10" t="s">
         <v>0</v>
       </c>
@@ -803,7 +800,7 @@
       </c>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
@@ -817,7 +814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
@@ -832,14 +829,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" s="10" t="s">
         <v>7</v>
       </c>
@@ -851,7 +848,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
         <v>8</v>
       </c>
@@ -865,7 +862,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>1</v>
       </c>
@@ -873,7 +870,7 @@
         <v>20</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -881,7 +878,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <v>20</v>
       </c>
@@ -897,14 +894,14 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B18" s="10" t="s">
         <v>11</v>
       </c>
@@ -915,7 +912,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
@@ -928,7 +925,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>8</v>
       </c>
@@ -941,7 +938,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <v>19</v>
       </c>
@@ -954,7 +951,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <v>20</v>
       </c>
@@ -967,13 +964,13 @@
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B25" s="10" t="s">
         <v>14</v>
       </c>
@@ -985,7 +982,7 @@
       <c r="J25" s="13"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B26" s="10" t="s">
         <v>8</v>
       </c>
@@ -1001,7 +998,7 @@
       </c>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
         <v>1</v>
       </c>
@@ -1019,7 +1016,7 @@
       </c>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <v>20</v>
       </c>
@@ -1037,7 +1034,7 @@
       </c>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
       <c r="I29" s="3">
         <v>20</v>
       </c>
@@ -1046,19 +1043,19 @@
       </c>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="7"/>
     </row>
-    <row r="33" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1068,142 +1065,142 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B35" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="13"/>
       <c r="I35" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="13"/>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B36" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F36" s="10"/>
       <c r="I36" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L36" s="10"/>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B37" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J36" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K36" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="L36" s="10"/>
-    </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="C37" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F37" s="10"/>
       <c r="I37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="L37" s="10"/>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B38" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J37" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="K37" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="L37" s="10"/>
-    </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B39" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>24</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F39" s="10"/>
       <c r="I39" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L39" s="10"/>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.35">
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="7"/>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:18" x14ac:dyDescent="0.35">
       <c r="N42" s="7"/>
       <c r="O42" s="7"/>
       <c r="P42" s="7"/>
       <c r="Q42" s="7"/>
       <c r="R42" s="7"/>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B43" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="J43" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K43" s="10"/>
       <c r="N43" s="7"/>
@@ -1212,16 +1209,16 @@
       <c r="Q43" s="7"/>
       <c r="R43" s="7"/>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B44" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="3" t="s">
         <v>9</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K44" s="3" t="s">
         <v>12</v>
@@ -1232,7 +1229,7 @@
       <c r="Q44" s="7"/>
       <c r="R44" s="7"/>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B45" s="3">
         <v>20</v>
       </c>
@@ -1243,7 +1240,7 @@
         <v>5</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K45" s="3" t="s">
         <v>12</v>
@@ -1254,7 +1251,7 @@
       <c r="Q45" s="7"/>
       <c r="R45" s="7"/>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B46" s="3">
         <v>40</v>
       </c>
@@ -1276,7 +1273,7 @@
       <c r="Q46" s="7"/>
       <c r="R46" s="7"/>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:18" x14ac:dyDescent="0.35">
       <c r="J47" s="3">
         <v>45</v>
       </c>
@@ -1289,42 +1286,44 @@
       <c r="Q47" s="7"/>
       <c r="R47" s="7"/>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="L48" s="7"/>
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
       <c r="P48" s="7"/>
       <c r="Q48" s="7"/>
       <c r="R48" s="7"/>
     </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="L49" s="7"/>
       <c r="N49" s="7"/>
       <c r="O49" s="7"/>
       <c r="P49" s="7"/>
       <c r="Q49" s="7"/>
       <c r="R49" s="7"/>
     </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B50" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C50" s="10"/>
-      <c r="J50" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="K50" s="10"/>
-      <c r="L50" s="10"/>
+      <c r="J50" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K50" s="13"/>
+      <c r="L50" s="7"/>
       <c r="N50" s="7"/>
       <c r="O50" s="7"/>
       <c r="P50" s="7"/>
       <c r="Q50" s="7"/>
       <c r="R50" s="7"/>
     </row>
-    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B51" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J51" s="3" t="s">
         <v>8</v>
@@ -1332,21 +1331,19 @@
       <c r="K51" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L51" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="L51" s="7"/>
       <c r="N51" s="7"/>
       <c r="O51" s="7"/>
       <c r="P51" s="7"/>
       <c r="Q51" s="7"/>
       <c r="R51" s="7"/>
     </row>
-    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B52" s="3">
         <v>20</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>8</v>
@@ -1354,21 +1351,19 @@
       <c r="K52" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L52" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="L52" s="7"/>
       <c r="N52" s="7"/>
       <c r="O52" s="7"/>
       <c r="P52" s="7"/>
       <c r="Q52" s="7"/>
       <c r="R52" s="7"/>
     </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B53" s="3">
         <v>40</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J53" s="3">
         <v>20</v>
@@ -1376,47 +1371,43 @@
       <c r="K53" s="3">
         <v>24</v>
       </c>
-      <c r="L53" s="3">
-        <v>24</v>
-      </c>
+      <c r="L53" s="7"/>
       <c r="N53" s="7"/>
       <c r="O53" s="7"/>
       <c r="P53" s="7"/>
       <c r="Q53" s="7"/>
       <c r="R53" s="7"/>
     </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:18" x14ac:dyDescent="0.35">
       <c r="J54" s="3">
         <v>40</v>
       </c>
       <c r="K54" s="3">
         <v>44</v>
       </c>
-      <c r="L54" s="3">
-        <v>44</v>
-      </c>
+      <c r="L54" s="7"/>
       <c r="N54" s="7"/>
       <c r="O54" s="7"/>
       <c r="P54" s="7"/>
       <c r="Q54" s="7"/>
       <c r="R54" s="7"/>
     </row>
-    <row r="55" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="56" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B56" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
       <c r="I56" s="6"/>
       <c r="J56" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K56" s="10"/>
     </row>
-    <row r="57" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B57" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="3" t="s">
@@ -1424,13 +1415,13 @@
       </c>
       <c r="I57" s="6"/>
       <c r="J57" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K57" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B58" s="3">
         <v>20</v>
       </c>
@@ -1442,13 +1433,13 @@
       </c>
       <c r="I58" s="6"/>
       <c r="J58" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K58" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B59" s="3">
         <v>40</v>
       </c>
@@ -1466,7 +1457,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="I60" s="6"/>
       <c r="J60" s="3">
         <v>45</v>
@@ -1475,42 +1466,42 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
     </row>
-    <row r="62" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
       <c r="O62" s="6"/>
       <c r="P62" s="6"/>
     </row>
-    <row r="63" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B63" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
       <c r="I63" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J63" s="10"/>
       <c r="K63" s="6"/>
       <c r="O63" s="6"/>
       <c r="P63" s="6"/>
     </row>
-    <row r="64" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B64" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D64" s="10"/>
       <c r="I64" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J64" s="3" t="s">
         <v>12</v>
@@ -1519,7 +1510,7 @@
       <c r="O64" s="6"/>
       <c r="P64" s="6"/>
     </row>
-    <row r="65" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B65" s="3">
         <v>1</v>
       </c>
@@ -1527,7 +1518,7 @@
         <v>13</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I65" s="3" t="s">
         <v>8</v>
@@ -1539,7 +1530,7 @@
       <c r="O65" s="6"/>
       <c r="P65" s="6"/>
     </row>
-    <row r="66" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B66" s="3">
         <v>2</v>
       </c>
@@ -1547,7 +1538,7 @@
         <v>13</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I66" s="3">
         <v>1</v>
@@ -1559,7 +1550,7 @@
       <c r="O66" s="6"/>
       <c r="P66" s="6"/>
     </row>
-    <row r="67" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:16" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="I67" s="3">
         <v>2</v>
       </c>
@@ -1567,13 +1558,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:16" x14ac:dyDescent="0.35">
       <c r="I68" s="6"/>
       <c r="J68" s="6"/>
     </row>
-    <row r="69" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B69" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -1583,18 +1574,18 @@
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="72" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B72" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C72" s="10"/>
       <c r="I72" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J72" s="10"/>
     </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B73" s="3" t="s">
         <v>1</v>
       </c>
@@ -1605,29 +1596,29 @@
         <v>8</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B74" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I74" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B75" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I75" s="3">
         <v>100</v>
@@ -1636,9 +1627,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B78" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
@@ -1648,20 +1639,20 @@
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
     </row>
-    <row r="79" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="80" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B80" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C80" s="10"/>
       <c r="I80" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J80" s="10"/>
       <c r="K80" s="10"/>
       <c r="L80" s="10"/>
     </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B81" s="3" t="s">
         <v>1</v>
       </c>
@@ -1669,45 +1660,45 @@
         <v>2</v>
       </c>
       <c r="I81" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J81" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J81" s="3" t="s">
+      <c r="K81" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="K81" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B82" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D82" s="1"/>
       <c r="I82" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J82" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J82" s="3" t="s">
+      <c r="K82" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="K82" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="L82" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B83" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D83" s="1"/>
       <c r="I83" s="3">
@@ -1723,35 +1714,35 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="86" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="87" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="I87" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J87" s="10"/>
       <c r="K87" s="10"/>
       <c r="L87" s="10"/>
     </row>
-    <row r="88" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B88" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C88" s="10"/>
       <c r="I88" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J88" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J88" s="3" t="s">
+      <c r="K88" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="K88" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="L88" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B89" s="3" t="s">
         <v>1</v>
       </c>
@@ -1759,24 +1750,24 @@
         <v>2</v>
       </c>
       <c r="I89" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J89" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J89" s="3" t="s">
+      <c r="K89" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="K89" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="L89" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B90" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I90" s="3">
         <v>5</v>
@@ -1788,22 +1779,22 @@
         <v>96</v>
       </c>
       <c r="L90" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="91" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B91" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="92" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="93" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="96" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B96" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
@@ -1813,19 +1804,19 @@
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B98" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C98" s="10"/>
       <c r="D98" s="10"/>
       <c r="I98" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J98" s="10"/>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B99" s="10" t="s">
         <v>8</v>
       </c>
@@ -1838,7 +1829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B100" s="3">
         <v>1</v>
       </c>
@@ -1846,7 +1837,7 @@
         <v>20</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I100" s="3" t="s">
         <v>8</v>
@@ -1855,7 +1846,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B101" s="3">
         <v>40</v>
       </c>
@@ -1863,7 +1854,7 @@
         <v>50</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I101" s="3">
         <v>19</v>
@@ -1872,7 +1863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B102" s="3">
         <v>50</v>
       </c>
@@ -1880,7 +1871,7 @@
         <v>60</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I102" s="3">
         <v>45</v>
@@ -1889,7 +1880,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -1902,7 +1893,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -1914,7 +1905,7 @@
       <c r="K104" s="7"/>
       <c r="L104" s="7"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -1925,7 +1916,7 @@
       <c r="J105" s="7"/>
       <c r="K105" s="7"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -1937,7 +1928,7 @@
       <c r="K106" s="7"/>
       <c r="L106" s="7"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -1949,21 +1940,21 @@
       <c r="K107" s="7"/>
       <c r="L107" s="7"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
       <c r="K108" s="7"/>
       <c r="L108" s="7"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
       <c r="K109" s="7"/>
       <c r="L109" s="7"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
@@ -1977,10 +1968,10 @@
     <mergeCell ref="K36:L36"/>
     <mergeCell ref="K37:L37"/>
     <mergeCell ref="K39:L39"/>
+    <mergeCell ref="J50:K50"/>
     <mergeCell ref="I87:L87"/>
     <mergeCell ref="I80:L80"/>
     <mergeCell ref="B50:C50"/>
-    <mergeCell ref="J50:L50"/>
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="J56:K56"/>
     <mergeCell ref="B57:C57"/>
@@ -2023,7 +2014,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2035,7 +2026,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>